<commit_message>
Load descriptions from spreadsheet.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F321838E-DD31-45FD-BCD4-4027746D77B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553B1868-FE83-478D-85BB-1EADF9A6476E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CAPABILITIES" sheetId="1" r:id="rId1"/>
+    <sheet name="META" sheetId="2" r:id="rId1"/>
+    <sheet name="CAPABILITIES" sheetId="1" r:id="rId2"/>
+    <sheet name="DESCRIPTIONS" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
   <si>
     <t>capability_id</t>
   </si>
@@ -82,9 +84,6 @@
     <t>CA</t>
   </si>
   <si>
-    <t>countable</t>
-  </si>
-  <si>
     <t>IDF Regts</t>
   </si>
   <si>
@@ -284,6 +283,24 @@
   </si>
   <si>
     <t>DF Regt</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Proin ac est et ante sagittis volutpat vel non nunc. Nunc gravida est ex, elementum tincidunt enim accumsan at. Fusce vel tempor lorem. Nunc a nulla nulla. Sed faucibus, erat et iaculis dapibus, ligula lacus iaculis tellus, a tempus ex urna vel magna. Donec eu metus eu ante dignissim blandit non vitae mi. In metus massa, congue sed massa nec, aliquam gravida nisi. Nam ornare, ante ac tempor maximus, velit enim rhoncus ligula, vitae pretium neque nunc eget erat. Nullam aliquet lectus vitae massa eleifend, vitae mattis mi sollicitudin. Maecenas sed mollis sem. Proin et magna ultrices, ultricies mauris at, elementum risus. Nullam aliquam fermentum mi tincidunt pulvinar.</t>
+  </si>
+  <si>
+    <t>Praesent eu sapien maximus, vulputate sapien vel, iaculis mauris. Suspendisse erat odio, tristique vel ligula sed, rutrum egestas mauris. Donec non maximus sem. Quisque ornare, ligula ut bibendum vestibulum, nulla dolor volutpat quam, congue finibus dui tellus non metus. Mauris euismod, metus vitae feugiat bibendum, nisi leo condimentum mi, et ultricies erat felis vitae purus. Donec tortor nulla, laoreet in tristique non, pharetra ultrices tortor. Nulla tempus tortor non sapien tincidunt, eu imperdiet lacus dignissim. Proin id orci libero. Phasellus mattis tempor velit, non vestibulum libero fermentum sed. Curabitur tincidunt ipsum non luctus dapibus. Curabitur et vehicula justo. Mauris ut purus pharetra, porttitor ex vel, venenatis urna. Vivamus ornare urna eu arcu euismod, vel volutpat mauris pulvinar. Nam elementum dui at velit sollicitudin hendrerit.</t>
+  </si>
+  <si>
+    <t>nterdum et malesuada fames ac ante ipsum primis in faucibus. Nam quis gravida lacus, quis gravida neque. Morbi hendrerit turpis ac mollis venenatis. Donec ac ullamcorper nisl. In hac habitasse platea dictumst. Cras tempor posuere bibendum. Vivamus consectetur accumsan dolor quis eleifend. Quisque quis magna mauris.</t>
   </si>
 </sst>
 </file>
@@ -773,11 +790,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1132,11 +1152,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BED6CC-3CF3-433E-8744-62651D8DEA7F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,6 +1183,7 @@
     <col min="11" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1211,13 +1244,13 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
@@ -1256,7 +1289,7 @@
         <v>100</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q2" s="2">
         <v>25</v>
@@ -1267,13 +1300,13 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -1312,7 +1345,7 @@
         <v>100</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="2">
         <v>25</v>
@@ -1323,13 +1356,13 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
@@ -1368,7 +1401,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q4" s="2">
         <v>25</v>
@@ -1379,13 +1412,13 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
@@ -1424,7 +1457,7 @@
         <v>100</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q5" s="2">
         <v>25</v>
@@ -1435,13 +1468,13 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
@@ -1480,7 +1513,7 @@
         <v>100</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q6" s="2">
         <v>0</v>
@@ -1491,16 +1524,16 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="1">
         <v>1000</v>
@@ -1535,8 +1568,8 @@
       <c r="O7" s="1">
         <v>100</v>
       </c>
-      <c r="P7" t="s">
-        <v>20</v>
+      <c r="P7" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q7">
         <v>25</v>
@@ -1547,16 +1580,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1">
         <v>1800</v>
@@ -1591,8 +1624,8 @@
       <c r="O8" s="1">
         <v>100</v>
       </c>
-      <c r="P8" t="s">
-        <v>20</v>
+      <c r="P8" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q8">
         <v>25</v>
@@ -1603,16 +1636,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E9" s="3">
         <v>700</v>
@@ -1648,7 +1681,7 @@
         <v>100</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q9" s="2">
         <v>25</v>
@@ -1659,16 +1692,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" s="3">
         <v>1300</v>
@@ -1704,7 +1737,7 @@
         <v>100</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q10" s="2">
         <v>25</v>
@@ -1715,16 +1748,16 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11" s="3">
         <v>900</v>
@@ -1760,7 +1793,7 @@
         <v>100</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q11" s="2">
         <v>25</v>
@@ -1771,16 +1804,16 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="3">
         <v>1400</v>
@@ -1816,7 +1849,7 @@
         <v>100</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="2">
         <v>0</v>
@@ -1827,16 +1860,16 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="3">
         <v>200</v>
@@ -1872,7 +1905,7 @@
         <v>100</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q13" s="2">
         <v>0</v>
@@ -1883,16 +1916,16 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="3">
         <v>300</v>
@@ -1928,7 +1961,7 @@
         <v>100</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q14" s="2">
         <v>0</v>
@@ -1939,16 +1972,16 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" s="3">
         <v>400</v>
@@ -1984,7 +2017,7 @@
         <v>100</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q15" s="2">
         <v>0</v>
@@ -1995,16 +2028,16 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="3">
         <v>1400</v>
@@ -2040,7 +2073,7 @@
         <v>100</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q16" s="2">
         <v>0</v>
@@ -2051,16 +2084,16 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E17" s="3">
         <v>1800</v>
@@ -2096,7 +2129,7 @@
         <v>100</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q17" s="2">
         <v>0</v>
@@ -2107,16 +2140,16 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="3">
         <v>1200</v>
@@ -2152,7 +2185,7 @@
         <v>100</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="Q18" s="2">
         <v>25</v>
@@ -2163,16 +2196,16 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>61</v>
-      </c>
-      <c r="D19" t="s">
-        <v>62</v>
       </c>
       <c r="E19" s="1">
         <v>40</v>
@@ -2207,8 +2240,8 @@
       <c r="O19" s="1">
         <v>100</v>
       </c>
-      <c r="P19" t="s">
-        <v>20</v>
+      <c r="P19" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2219,16 +2252,16 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1">
         <v>300</v>
@@ -2263,8 +2296,8 @@
       <c r="O20" s="1">
         <v>100</v>
       </c>
-      <c r="P20" t="s">
-        <v>20</v>
+      <c r="P20" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2275,16 +2308,16 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="1">
         <v>2800</v>
@@ -2319,8 +2352,8 @@
       <c r="O21" s="1">
         <v>100</v>
       </c>
-      <c r="P21" t="s">
-        <v>20</v>
+      <c r="P21" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2331,16 +2364,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
         <v>67</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="1">
         <v>300</v>
@@ -2375,8 +2408,8 @@
       <c r="O22" s="1">
         <v>100</v>
       </c>
-      <c r="P22" t="s">
-        <v>20</v>
+      <c r="P22" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2387,13 +2420,13 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3">
@@ -2430,13 +2463,64 @@
         <v>100</v>
       </c>
       <c r="P23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137E404D-16B9-47BF-83EA-36E59F036C91}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="2" max="2" width="105.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="114.140625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="2">
-        <v>0</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0</v>
+      <c r="B3" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6 - added overhead to all capabilities.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B695EC-80E3-45AE-89AD-18587D90D420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408610B8-3359-461A-97A7-3AA100309C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VARS" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
   <si>
     <t>capability_id</t>
   </si>
@@ -294,15 +294,6 @@
     <t>fr</t>
   </si>
   <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Proin ac est et ante sagittis volutpat vel non nunc. Nunc gravida est ex, elementum tincidunt enim accumsan at. Fusce vel tempor lorem. Nunc a nulla nulla. Sed faucibus, erat et iaculis dapibus, ligula lacus iaculis tellus, a tempus ex urna vel magna. Donec eu metus eu ante dignissim blandit non vitae mi. In metus massa, congue sed massa nec, aliquam gravida nisi. Nam ornare, ante ac tempor maximus, velit enim rhoncus ligula, vitae pretium neque nunc eget erat. Nullam aliquet lectus vitae massa eleifend, vitae mattis mi sollicitudin. Maecenas sed mollis sem. Proin et magna ultrices, ultricies mauris at, elementum risus. Nullam aliquam fermentum mi tincidunt pulvinar.</t>
-  </si>
-  <si>
-    <t>Praesent eu sapien maximus, vulputate sapien vel, iaculis mauris. Suspendisse erat odio, tristique vel ligula sed, rutrum egestas mauris. Donec non maximus sem. Quisque ornare, ligula ut bibendum vestibulum, nulla dolor volutpat quam, congue finibus dui tellus non metus. Mauris euismod, metus vitae feugiat bibendum, nisi leo condimentum mi, et ultricies erat felis vitae purus. Donec tortor nulla, laoreet in tristique non, pharetra ultrices tortor. Nulla tempus tortor non sapien tincidunt, eu imperdiet lacus dignissim. Proin id orci libero. Phasellus mattis tempor velit, non vestibulum libero fermentum sed. Curabitur tincidunt ipsum non luctus dapibus. Curabitur et vehicula justo. Mauris ut purus pharetra, porttitor ex vel, venenatis urna. Vivamus ornare urna eu arcu euismod, vel volutpat mauris pulvinar. Nam elementum dui at velit sollicitudin hendrerit.</t>
-  </si>
-  <si>
-    <t>Interdum et malesuada fames ac ante ipsum primis in faucibus. Nam quis gravida lacus, quis gravida neque. Morbi hendrerit turpis ac mollis venenatis. Donec ac ullamcorper nisl. In hac habitasse platea dictumst. Cras tempor posuere bibendum. Vivamus consectetur accumsan dolor quis eleifend. Quisque quis magna mauris.</t>
-  </si>
-  <si>
     <t>Value (or en)</t>
   </si>
   <si>
@@ -315,61 +306,142 @@
     <t>report_poster_url</t>
   </si>
   <si>
-    <t>https://pbo-dpb--static-statique--dev.s3.ca-central-1.amazonaws.com/images/3886459ef1d1498a3bfb96fa07d030f0c1986f90f7ea8465b2d2c81087a2f1af</t>
-  </si>
-  <si>
-    <t>https://pbo-dpb--static-statique--dev.s3.ca-central-1.amazonaws.com/images/ae3f760fcccf4fb8e9d8aa710372a4e620e608e608e9a7f7ca2bc1cfc54ce997</t>
-  </si>
-  <si>
-    <t>https://www.pbo-dpb.ca/en/lorem-ipsum</t>
-  </si>
-  <si>
-    <t>https://www.pbo-dpb.ca/fr/lorem-ipsum</t>
-  </si>
-  <si>
-    <t>intro</t>
-  </si>
-  <si>
-    <t>This tool details the development of a framework to address the costs of military capabilities and the potential trade-offs implied should a government policy require the adjustment of the structure of the Canadian Armed Forces.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cet outil détaille l’élaboration d’un cadre permettant d’aborder les coûts des capacités militaires et les compromis potentiels qu’impliquerait une politique gouvernementale exigeant l’ajustement de la structure des Forces armées canadiennes.  </t>
-  </si>
-  <si>
-    <t>capabilities_rounding_note_cost</t>
-  </si>
-  <si>
-    <t>capabilities_rounding_note_personnel</t>
-  </si>
-  <si>
-    <t>Costs are rounded to the nearest 10 million (10 000 000).</t>
-  </si>
-  <si>
-    <t>Les coûts sont arrondis à la dizaine de millions la plus proche (10 000 000).</t>
-  </si>
-  <si>
-    <t>Personnel is rounded to the nearest 100, with one exception: AOPV is &lt;100, so we round to the nearest 10.</t>
-  </si>
-  <si>
-    <t>Les effectifs sont arrondis à la centaine la plus proche, à une exception près : comme il y a moins de 100 navires de patrouille extracôtiers de l'Arctique, cette capacité est arrondie à la dizaine la plus proche.</t>
-  </si>
-  <si>
-    <t>Costs are rounded to the nearest 100 million (100 000 000).</t>
-  </si>
-  <si>
-    <t>Les coûts sont arrondis à la centaine de millions la plus proche (100 000 000).</t>
-  </si>
-  <si>
-    <t>overhead_and_totals_rounding_note_personnel</t>
-  </si>
-  <si>
-    <t>Personnel is rounded to the nearest 1000.</t>
-  </si>
-  <si>
-    <t>Les effectifs sont arrondis au millier le plus proche.</t>
-  </si>
-  <si>
-    <t>overhead_and_totals_rounding_note_cost</t>
+    <t>The Canadian Rangers are a sub-component of the Canadian Army Reserve who live and work in remote, isolated, and coastal regions of Canada. They are knowledgeable of their remote lands and communities, and provide light-equipped, self-sufficient mobile forces within Canada.</t>
+  </si>
+  <si>
+    <t>Direct fire regiments are heavily armoured land units supported by reconnaissance and light armour. Their primary weapon systems are the Leopard 2 Family of Vehicles and the Light Armoured Vehicle (LAV).</t>
+  </si>
+  <si>
+    <t>Indirect fire regiments use land weapon systems to engage a target not visible to the weapon operator due to distance, terrain, weather, or obscurants. Their primary weapon systems are the M777 Lightweight 155-mm Towed Howitzer and the 81-mm Mortar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Light infantry battalions are mobile soldiers that can operate without transportation or mechanized support. </t>
+  </si>
+  <si>
+    <t>Mechanized infantry battalions are mobile soldiers that are intended to operate with mobile land transportation. They operate lightly armoured vehicles and personnel carriers often with mounted land weapons systems.</t>
+  </si>
+  <si>
+    <t>The CF Information Operations Group operates satellites, cyber operations, and electronic warfare to achieve or promote specific military objectives over specific adversaries.</t>
+  </si>
+  <si>
+    <t>Special Operations is a high-readiness organization able to deploy agile forces on very short notice against threats at home and abroad. They recruit directly from the Canadian Armed Forces Regular and Reserve Forces and further develop their skills with specialized equipment distinct from all other military capabilities.</t>
+  </si>
+  <si>
+    <t>Air transport capability is used for a wide range of missions, including troop transport, tactical airlift, freight, and medical transport. It can land and airdrop heavy loads of equipment, supplies and personnel into hostile environments. Assets associated with this capability include the CC-130J Hercules and CC-150 Polaris.</t>
+  </si>
+  <si>
+    <t>Fixed-wing search and rescue units operate conventional aircraft with longer ranges and carrying capacities than helicopters. They tend to be used in the initial phases of the search to locate people and equipment in distress. The primary fixed-wing aircraft used for this capability is the CC-130H Hercules, with a new fleet of CC-295 Kingfishers expected to take over by the end of the current decade.</t>
+  </si>
+  <si>
+    <t>Maritime helicopters are used for surface and sub-surface surveillance, search and rescue missions, tactical transport and more. They can operate in most weather conditions to provide air support to the Royal Canadian Navy and can be launched directly from ships. The Royal Canadian Air Force employs the CH-148 Cyclone in this role.</t>
+  </si>
+  <si>
+    <t>Maritime patrol aircraft are long range aircraft that support a variety of roles, including operations management, surveillance and reconnaissance, anti-submarine and anti-surface warfare, and strike coordination. It can also assist other government agencies to combat illegal fishing, pollution, drug trafficking, and more. The CP-140 Aurora is currently the Air Force’s maritime patrol aircraft.</t>
+  </si>
+  <si>
+    <t>Medium and heavy life helicopters are used to transport equipment and personnel during domestic or deployed operations. They have enhanced self-protection capabilities, including anti-missile protection systems, radar as well as laser warning systems, ballistic protection, and self-defence machine guns. The CH-147F Chinook is employed in this role.</t>
+  </si>
+  <si>
+    <t>The North American Aerospace Defence Command (NORAD) is a Canadian-American bi-national organization charged with the missions of aerospace warning, aerospace control, and maritime warning for North America. Aerospace warning includes the detection, validation, and warning of attack against North America whether by aircraft, missiles, or space vehicles. Canada’s most significant contribution is the North Warning System (NWS), a chain of radar stations that provides aerospace surveillance of Canadian and United States northern approaches. Using a series of long and short-range air defence radar sites, the NWS enables Canada’s situational awareness of who and what is entering Canadian airspace from the north.</t>
+  </si>
+  <si>
+    <t>Search and Rescue helicopters operate helicopters that are more agile and maneuverable than fixed wing aircraft. They can operate closer to the ground in extreme Canadian conditions while providing some range and lift capabilities. The CH-149 Cormorant is used in this role.</t>
+  </si>
+  <si>
+    <t>Strategic airlift is used to haul large quantities of cargo and personnel over long distances. They are equipped with advanced digital avionics and can land in remote airfields. One of these aircraft can haul three CH-146 Griffon helicopters with refuelling tanks, or up to 102 paratroopers. The Royal Canadian Air Force’s strategic airlift platform is the CC-177 Globemaster III.</t>
+  </si>
+  <si>
+    <t>Tactical aviation continuously supports ground forces, and in the RCAF they exclusively operate helicopters. They carry personnel and materiel over shorter distances and are more agile aircraft with self-defence weapons, a powerful searchlight, and a hoist to extract people and cargo from almost any terrain. The CH-146 Griffon fills this role for the Royal Canadian Air Force.</t>
+  </si>
+  <si>
+    <t>Tactical fighters are extremely high speed and lethal air weapons system that can perform capabilities such as air defence, ground attack, and tactical support. The CF-188 Hornet is the Royal Canadian Air Force’s current tactical fighter, with the F-35A Lightning II slated to gradually replace this fleet over the next 10 years.</t>
+  </si>
+  <si>
+    <t>The Harry DeWolf-class Arctic offshore patrol vessels (AOPV) operate along Canada’s coast especially in the Arctic with its ability to break new ice. They conduct armed surveillance operations, contribute to emergency responses and, and conduct search and rescue missions. They can also launch maritime helicopters.</t>
+  </si>
+  <si>
+    <t>The Kingston-class coastal defence vessels conduct coastal surveillance and patrol. Coastal surveillance involves general naval operations and exercises, search and rescue, law enforcement, resource protection, and fisheries patrols. The ships can be fitted for route survey, bottom object inspection, and mine hunting and countermeasure.</t>
+  </si>
+  <si>
+    <t>The Halifax-class frigates were originally designed for anti-submarine warfare and anti-surface warfare, primarily in the open ocean environment. They are now the primary warships of the RCN, with modernization projects updating the radar, communications, and weapons systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Victoria-class submarines are extremely quiet and stealthy vessels capable of underwater operations. They can conduct operations around the world including in the Arctic, and provide support to maritime law-enforcement, narcotics trafficking, smuggling, and polluting cases. </t>
+  </si>
+  <si>
+    <t>Les Rangers canadiens sont une sous-composante de la Réserve des Forces armées canadiennes; ils vivent et travaillent dans des régions éloignées, isolées et côtières du pays. Outre leur connaissance des terres et des communautés éloignées, ils fournissent des forces mobiles autosuffisantes dotées d’équipement léger à l’intérieur du Canada.</t>
+  </si>
+  <si>
+    <t>Les régiments de tir direct sont des unités terrestres blindées lourdes qui sont appuyées par des forces de reconnaissance et des véhicules blindés légers. Leurs systèmes d’armes principaux sont la famille de véhicules Léopard 2 et les véhicules blindés légers.</t>
+  </si>
+  <si>
+    <t>Les régiments de tir indirect utilisent des systèmes d'armes terrestres pour engager un objectif qui n’est pas visible par l’utilisateur de l'arme en raison de la distance, du terrain, des conditions météorologiques ou d’obscurcissants. Leurs principaux systèmes d’armes sont l’obusier tracté léger M777 de 155 mm et le mortier de 81 mm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les bataillons d’infanterie légère sont des soldats mobiles qui peuvent opérer sans transport ni soutien mécanisé. </t>
+  </si>
+  <si>
+    <t>Les bataillons d’infanterie mécanisés sont des soldats mobiles qui opèrent avec des moyens mobiles de transport terrestre. Ils utilisent des véhicules blindés légers et des véhicules de transport de personnel, souvent équipés de systèmes d’armes terrestres montés.</t>
+  </si>
+  <si>
+    <t>Le Groupe des opérations d’information des FC utilise des satellites, des cyberopérations et la guerre électronique afin d’atteindre ou de promouvoir des objectifs militaires définis face à des adversaires précis.</t>
+  </si>
+  <si>
+    <t>Les opérations spéciales sont une organisation à disponibilité opérationnelle élevée qui est capable de déployer des forces agiles dans un délai très court afin de contrer des menaces au Canada et à l’étranger. Elles recrutent directement au sein des forces régulières et de réserve des Forces armées canadiennes et développent leurs compétences à l'aide d’équipements spécialisés distincts de toutes les autres capacités militaires.</t>
+  </si>
+  <si>
+    <t>La capacité de transport aérien est utilisée pour un large éventail de missions, notamment le transport de troupes, le transport aérien tactique, le transport de fret et le transport médical. Elle peut permettre d’atterrir dans des milieux inhospitaliers et d’y larguer de lourdes charges d’équipement et de provisions, ainsi que du personnel. Les moyens associés à cette capacité sont le CC-130J Hercules et le CC-150 Polaris.</t>
+  </si>
+  <si>
+    <t>Les unités de recherche et de sauvetage à voilure fixe utilisent des aéronefs conventionnels dont le rayon d'action et la capacité de transport sont plus importants que ceux des hélicoptères. EIles sont généralement utilisées dans les phases initiales de la recherche pour repérer l’équipement et les personnes en détresse. Le principal aéronef à voilure fixe utilisé pour cette capacité est le CC-130H Hercules. Une nouvelle flotte de CC-295 Kingfishers devrait prendre le relais d’ici la fin de la décennie.</t>
+  </si>
+  <si>
+    <t>Les hélicoptères maritimes sont utilisés pour la surveillance en surface et la surveillance sous-marine, les missions de recherche et de sauvetage, le transport tactique, etc. Ils peuvent opérer dans la plupart des conditions météorologiques pour fournir un soutien aérien à la Marine royale canadienne et peuvent être lancés directement à partir de navires. L’Aviation royale canadienne utilise le CH-148 Cyclone dans ce rôle.</t>
+  </si>
+  <si>
+    <t>Les aéronefs de patrouille maritime sont des appareils à long rayon d’action qui remplissent diverses fonctions, notamment la gestion des opérations, la surveillance et la reconnaissance, la lutte anti-sous-marins et antinavires, ainsi que la coordination des attaques. Ils peuvent aussi aider d’autres organisations gouvernementales à lutter contre la pêche illégale, la pollution, le trafic de stupéfiants, etc. Le CP-140 Aurora est actuellement l’aéronef de patrouille maritime de l’Aviation royale canadienne.</t>
+  </si>
+  <si>
+    <t>Les hélicoptères moyens et lourds sont utilisés pour transporter du matériel et du personnel dans le cadre d’opérations nationales ou de déploiement. Ils disposent de capacités d’autoprotection renforcées, y compris de systèmes de protection antimissile, de systèmes d’alerte radar et laser, de protection balistique et de mitrailleuses d’autodéfense. Le CH-147F Chinook est employé dans ce rôle.</t>
+  </si>
+  <si>
+    <t>Le Commandement de la défense aérospatiale de l’Amérique du Nord (NORAD) est une organisation binationale canado-américaine chargée des missions d’alerte aérospatiale et maritime et de contrôle aérospatial de l’Amérique du Nord. L’alerte aérospatiale comprend la détection, la confirmation et l’avertissement de toute attaque contre l’Amérique du Nord par des aéronefs, des missiles ou des engins spatiaux. La contribution la plus importante du Canada est le Système d’alerte du Nord (NWS), une chaîne de stations radar qui assure la surveillance aérospatiale des approches nordiques du Canada et des États-Unis. Grâce à une série de sites radar de défense aérienne à longue et courte portée, le NWS permet au Canada de savoir qui et quoi pénètre dans son espace aérien depuis le nord.</t>
+  </si>
+  <si>
+    <t>Les hélicoptères de recherche et de sauvetage sont plus agiles et plus manœuvrables que les aéronefs à voilure fixe. Ils peuvent opérer plus près du sol dans des conditions canadiennes extrêmes tout en offrant un certain rayon d’action et certaines capacités de transport. Le CH-149 Cormorant est utilisé dans ce rôle.</t>
+  </si>
+  <si>
+    <t>Le transport aérien stratégique sert à transporter de grandes quantités de marchandises et de personnel sur de longues distances. Les appareils utilisés à cette fin sont équipés d’un système d’avionique numérique avancé et peuvent atterrir sur des aérodromes éloignés. Chacun peut transporter trois hélicoptères CH-146 Griffon et des réservoirs de ravitaillement, ou jusqu’à 102 parachutistes. La plateforme de transport aérien stratégique de l'Aviation royale canadienne est le CC-177 Globemaster III.</t>
+  </si>
+  <si>
+    <t>L’aviation tactique soutient en permanence les forces terrestres; dans l’ARC, elle utilise exclusivement des hélicoptères. Ses appareils transportent du personnel et du matériel sur de courtes distances et sont plus agiles. Ils sont équipés d’armes d'autodéfense, d’un puissant projecteur et d’un treuil permettant d’extraire des personnes et des biens de presque n’importe quel terrain. Le CH-146 Griffon remplit ce rôle pour l’Aviation royale canadienne.</t>
+  </si>
+  <si>
+    <t>Les chasseurs d’appui tactique sont des systèmes d’armes aériennes extrêmement rapides et létaux qui peuvent assurer des fonctions telles que la défense aérienne, l’attaque au sol et le soutien tactique. Le CF-188 Hornet est le chasseur d’appui tactique actuel de l’Aviation royale canadienne. Le F-35A Lightning II devrait le remplacer graduellement d’ici dix ans.</t>
+  </si>
+  <si>
+    <t>Les navires de patrouille extracôtiers et de l’Arctique (NPEA) de classe Harry DeWolf opèrent le long des côtes canadiennes, en particulier dans l’Arctique, où ils sont capables de briser la glace. Ils mènent des opérations de surveillance armée, contribuent aux interventions d’urgence et effectuent des missions de recherche et de sauvetage. Ils peuvent également lancer des hélicoptères maritimes.</t>
+  </si>
+  <si>
+    <t>Les navires de défense côtière de classe Kingston assurent la surveillance et la patrouille des côtes. La surveillance côtière comprend les opérations et les exercices navals généraux, la recherche et le sauvetage, l’application de la loi, la protection des ressources et la surveillance des pêches. Les navires peuvent être équipés pour le levé des fonds marins, l’inspection des objets de fond, la chasse aux mines et les contre-mesures.</t>
+  </si>
+  <si>
+    <t>Les frégates de classe Halifax ont été conçues à l’origine pour la lutte anti-sous-marins et antinavires, principalement en haute mer. Elles sont aujourd’hui les principaux navires de guerre de la MRC, et les projets de modernisation ont permis d’actualiser leurs systèmes de radar, de communication et d’armes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les sous-marins de classe Victoria sont des navires extrêmement silencieux et furtifs, capables de mener des opérations sous-marines. Ils peuvent mener des opérations dans le monde entier, y compris dans l’Arctique, et apporter leur soutien à l’application du droit maritime, à la lutte contre le trafic de stupéfiants, la contrebande et la pollution. </t>
+  </si>
+  <si>
+    <t>https://www.pbo-dpb.ca/en/publications/RP-2324-010-S--force-structure-model-canada-military-costs-personnel--un-modele-structure-forces-armee-canadienne-couts-personnel</t>
+  </si>
+  <si>
+    <t>https://www.pbo-dpb.ca/fr/publications/RP-2324-010-S--force-structure-model-canada-military-costs-personnel--un-modele-structure-forces-armee-canadienne-couts-personnel</t>
+  </si>
+  <si>
+    <t>https://distribution-i696d61676573.pbo-dpb.ca/fee2ba610188307b701bc95b8394489e4681c5af08aa93c6ffdc08df4fe6eb69</t>
+  </si>
+  <si>
+    <t>https://distribution-i696d61676573.pbo-dpb.ca/abfee44c6ef080b13520cd25d01512f70276f1b7398fcc67f4f884f31765f36d</t>
   </si>
 </sst>
 </file>
@@ -868,7 +940,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -882,9 +954,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1241,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BED6CC-3CF3-433E-8744-62651D8DEA7F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,96 +1325,42 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EABBE242-6CCE-4AA1-B459-C27072701204}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{3F684200-AAEB-4039-AF72-C7D401F7E9CF}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{52A3EFD2-5664-414E-9838-27B210767C3B}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{7454E9A6-D2F3-4CE1-AFBC-86F10F8587DD}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{55CCF2E8-9A0C-42C1-BB40-EBB6FDBD7110}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1354,7 +1369,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A2" sqref="A2:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,15 +2681,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137E404D-16B9-47BF-83EA-36E59F036C91}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="105.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="114.140625" style="2" customWidth="1"/>
   </cols>
@@ -2690,15 +2705,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2706,7 +2721,219 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added emerging capability note to AOPV.
</commit_message>
<xml_diff>
--- a/src/assets/payload.xlsx
+++ b/src/assets/payload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Downloads\dist\distfsm5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408610B8-3359-461A-97A7-3AA100309C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EC450F-7DBA-478E-A327-918F55ADC9A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-3285" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VARS" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>capability_id</t>
   </si>
@@ -138,24 +138,12 @@
     <t>Mar Helo</t>
   </si>
   <si>
-    <t>Maritime Helicopter (Sea King -&gt; Cyclone)</t>
-  </si>
-  <si>
     <t>MHelo</t>
   </si>
   <si>
-    <t>Medium/Heavy Lift Helicopter (CH-147)</t>
-  </si>
-  <si>
     <t>MPA</t>
   </si>
   <si>
-    <t>Maritime Patrol Aircraft (CP-140 Aurora)</t>
-  </si>
-  <si>
-    <t>Avion de patrouille maritime (CP-140 Aurora)</t>
-  </si>
-  <si>
     <t>NORAD</t>
   </si>
   <si>
@@ -165,15 +153,9 @@
     <t>SAR Helo</t>
   </si>
   <si>
-    <t>Search and Rescue Helicopter (CH-149)</t>
-  </si>
-  <si>
     <t>StratL</t>
   </si>
   <si>
-    <t>Strategic Airlift (C-17)</t>
-  </si>
-  <si>
     <t>Tact Avn</t>
   </si>
   <si>
@@ -195,9 +177,6 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>Air Transport (C-130, C-150)</t>
-  </si>
-  <si>
     <t>AOPV</t>
   </si>
   <si>
@@ -255,24 +234,9 @@
     <t>Aéronefs de recherche et sauvetage à voilure fixe</t>
   </si>
   <si>
-    <t>Hélicoptère maritime (Sea King -&gt; Cyclone)</t>
-  </si>
-  <si>
-    <t>Hélicoptère de transport moyen/lourd (CH-147)</t>
-  </si>
-  <si>
     <t>Défense aérospatiale nord-américaine</t>
   </si>
   <si>
-    <t>Hélicoptère de recherche et de sauvetage (CH-149)</t>
-  </si>
-  <si>
-    <t>Transport aérien stratégique (C-17)</t>
-  </si>
-  <si>
-    <t>Transport aérien (C-130, C-150)</t>
-  </si>
-  <si>
     <t>Navire de défense côtière</t>
   </si>
   <si>
@@ -442,6 +406,54 @@
   </si>
   <si>
     <t>https://distribution-i696d61676573.pbo-dpb.ca/abfee44c6ef080b13520cd25d01512f70276f1b7398fcc67f4f884f31765f36d</t>
+  </si>
+  <si>
+    <t>Air Transport</t>
+  </si>
+  <si>
+    <t>Transport aérien</t>
+  </si>
+  <si>
+    <t>Hélicoptère maritime</t>
+  </si>
+  <si>
+    <t>Maritime Helicopter</t>
+  </si>
+  <si>
+    <t>Long Range Patrol Aircraft</t>
+  </si>
+  <si>
+    <t>Aéronef de patrouille à long rayon</t>
+  </si>
+  <si>
+    <t>Medium/Heavy Lift Helicopter</t>
+  </si>
+  <si>
+    <t>Hélicoptère de transport moyen/lourd</t>
+  </si>
+  <si>
+    <t>Search and Rescue Helicopter</t>
+  </si>
+  <si>
+    <t>Hélicoptère de recherche et de sauvetage</t>
+  </si>
+  <si>
+    <t>Transport aérien stratégique</t>
+  </si>
+  <si>
+    <t>Strategic Airlift</t>
+  </si>
+  <si>
+    <t>specific_note_en</t>
+  </si>
+  <si>
+    <t>specific_note_fr</t>
+  </si>
+  <si>
+    <t>This capability is emerging. Costs will rise over the next 5 years.</t>
+  </si>
+  <si>
+    <t>Cette capacité est en cours de développement. Les coûts augmenteront au cours des cinq prochaines années.</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40BED6CC-3CF3-433E-8744-62651D8DEA7F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1325,32 +1337,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1366,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,9 +1397,11 @@
     <col min="13" max="14" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="51.28515625" customWidth="1"/>
+    <col min="20" max="20" width="47.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1442,16 +1456,22 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>140</v>
+      </c>
+      <c r="T1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -1490,7 +1510,7 @@
         <v>100</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="1">
         <v>25</v>
@@ -1499,7 +1519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1507,7 +1527,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -1546,7 +1566,7 @@
         <v>100</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="1">
         <v>25</v>
@@ -1555,7 +1575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1563,7 +1583,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -1602,7 +1622,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="1">
         <v>25</v>
@@ -1611,7 +1631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1619,7 +1639,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -1658,7 +1678,7 @@
         <v>100</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="1">
         <v>25</v>
@@ -1667,7 +1687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1714,7 +1734,7 @@
         <v>100</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q6" s="1">
         <v>0</v>
@@ -1723,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1731,7 +1751,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
@@ -1770,7 +1790,7 @@
         <v>100</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q7">
         <v>25</v>
@@ -1779,7 +1799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1787,7 +1807,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -1826,7 +1846,7 @@
         <v>100</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q8">
         <v>25</v>
@@ -1835,7 +1855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1843,7 +1863,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>36</v>
@@ -1882,7 +1902,7 @@
         <v>100</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q9" s="1">
         <v>25</v>
@@ -1891,15 +1911,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>36</v>
@@ -1938,7 +1958,7 @@
         <v>100</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q10" s="1">
         <v>25</v>
@@ -1947,15 +1967,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>134</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>36</v>
@@ -1994,7 +2014,7 @@
         <v>100</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q11" s="1">
         <v>25</v>
@@ -2003,15 +2023,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>36</v>
@@ -2050,7 +2070,7 @@
         <v>100</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="1">
         <v>0</v>
@@ -2059,15 +2079,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>36</v>
@@ -2106,7 +2126,7 @@
         <v>100</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="1">
         <v>0</v>
@@ -2115,15 +2135,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>136</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>36</v>
@@ -2162,7 +2182,7 @@
         <v>100</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q14" s="1">
         <v>0</v>
@@ -2171,15 +2191,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -2218,7 +2238,7 @@
         <v>100</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q15" s="1">
         <v>0</v>
@@ -2227,15 +2247,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>36</v>
@@ -2274,7 +2294,7 @@
         <v>100</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q16" s="1">
         <v>0</v>
@@ -2283,15 +2303,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>36</v>
@@ -2330,7 +2350,7 @@
         <v>100</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -2339,15 +2359,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>36</v>
@@ -2386,7 +2406,7 @@
         <v>100</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q18" s="1">
         <v>25</v>
@@ -2395,18 +2415,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5">
         <v>40</v>
@@ -2442,7 +2462,7 @@
         <v>100</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2450,19 +2470,25 @@
       <c r="R19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5">
         <v>300</v>
@@ -2498,7 +2524,7 @@
         <v>100</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -2507,18 +2533,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E21" s="5">
         <v>2800</v>
@@ -2554,7 +2580,7 @@
         <v>100</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -2563,18 +2589,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E22" s="5">
         <v>300</v>
@@ -2610,7 +2636,7 @@
         <v>100</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -2619,15 +2645,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="6">
@@ -2664,7 +2690,7 @@
         <v>100</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="Q23" s="1">
         <v>0</v>
@@ -2699,21 +2725,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2721,10 +2747,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2732,10 +2758,10 @@
         <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2743,10 +2769,10 @@
         <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2754,10 +2780,10 @@
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2765,10 +2791,10 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2776,10 +2802,10 @@
         <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -2787,10 +2813,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2798,142 +2824,142 @@
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>